<commit_message>
Finished all questions, minus the Challenge ones for now. Made bar chart to display needed data, but need to figure out how to display the Department when changing the data in the chart
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Barbie\Desktop\DA11\Excel\lookups-exercise-barbsjean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C8E804-F63B-420D-93F6-79D2F423D6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7575CEE5-C72E-43FA-B82C-778840869CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -333,9 +333,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -833,7 +834,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -846,6 +847,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -928,6 +930,1083 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Budget</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Vs Actual</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$A$84</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$B$83:$C$83</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Budget</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$B$84:$C$84</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>356640100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>341243679.13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8DE7-4005-8735-73A1D70690AA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$A$85</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FY18</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$B$83:$C$83</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Budget</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$B$85:$C$85</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>382685200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>346340810.81999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8DE7-4005-8735-73A1D70690AA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$B$83:$C$83</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Budget</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$B$86:$C$86</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>376548600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>355279492.22999901</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8DE7-4005-8735-73A1D70690AA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="23809567"/>
+        <c:axId val="312095903"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="23809567"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="312095903"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="312095903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="23809567"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79D50BBF-D857-6C20-7A31-EA482BBB17E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1273,8 +2352,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4373,15 +5452,15 @@
       <c r="A56" t="s">
         <v>24</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="10">
         <f>VLOOKUP(A56,$A$1:$P$52,4)</f>
         <v>-36209.630000000005</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="10">
         <f>VLOOKUP(A56,$A$1:$P$52,9)</f>
         <v>-27292.159999999974</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="10">
         <f>VLOOKUP(A56,$A$1:$P$52,14)</f>
         <v>-9181.0800000000163</v>
       </c>
@@ -4390,15 +5469,15 @@
       <c r="A57" t="s">
         <v>25</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="10">
         <f t="shared" ref="B57:B61" si="9">VLOOKUP(A57,$A$1:$P$52,4)</f>
         <v>0</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="10">
         <f t="shared" ref="C57:C61" si="10">VLOOKUP(A57,$A$1:$P$52,9)</f>
         <v>0</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="10">
         <f t="shared" ref="D57:D61" si="11">VLOOKUP(A57,$A$1:$P$52,14)</f>
         <v>-311228.08999999997</v>
       </c>
@@ -4407,15 +5486,15 @@
       <c r="A58" t="s">
         <v>32</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="10">
         <f t="shared" si="9"/>
         <v>-149396.10000000987</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="10">
         <f t="shared" si="10"/>
         <v>-189254.06000000006</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="10">
         <f t="shared" si="11"/>
         <v>-374962.91000000015</v>
       </c>
@@ -4424,15 +5503,15 @@
       <c r="A59" t="s">
         <v>38</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="10">
         <f t="shared" si="9"/>
         <v>-12230.810000000056</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="10">
         <f t="shared" si="10"/>
         <v>-45485.580000000075</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="10">
         <f t="shared" si="11"/>
         <v>-72.879999999888241</v>
       </c>
@@ -4441,15 +5520,15 @@
       <c r="A60" t="s">
         <v>39</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="10">
         <f t="shared" si="9"/>
         <v>-4950.4699999999721</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="10">
         <f t="shared" si="10"/>
         <v>-8005.7900000010268</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="10">
         <f t="shared" si="11"/>
         <v>-1724.9000000000233</v>
       </c>
@@ -4458,15 +5537,15 @@
       <c r="A61" t="s">
         <v>55</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="10">
         <f t="shared" si="9"/>
         <v>-184239.79000001028</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="10">
         <f t="shared" si="10"/>
         <v>-133456.33000001032</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="10">
         <f t="shared" si="11"/>
         <v>-82077.349999999627</v>
       </c>
@@ -4494,15 +5573,15 @@
       <c r="A65" t="s">
         <v>24</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="10">
         <f>_xlfn.XLOOKUP(A65,$A$1:$A$52,$D$1:$D$52)</f>
         <v>-36209.630000000005</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="10">
         <f>_xlfn.XLOOKUP(A65,$A$2:$A$52,$I$2:$I$52)</f>
         <v>-27292.159999999974</v>
       </c>
-      <c r="D65">
+      <c r="D65" s="10">
         <f>_xlfn.XLOOKUP(A65,$A$2:$A$52,$N$2:$N$52)</f>
         <v>-9181.0800000000163</v>
       </c>
@@ -4511,15 +5590,15 @@
       <c r="A66" t="s">
         <v>25</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="10">
         <f t="shared" ref="B66:B70" si="12">_xlfn.XLOOKUP(A66,$A$1:$A$52,$D$1:$D$52)</f>
         <v>0</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="10">
         <f t="shared" ref="C66:C70" si="13">_xlfn.XLOOKUP(A66,$A$2:$A$52,$I$2:$I$52)</f>
         <v>0</v>
       </c>
-      <c r="D66">
+      <c r="D66" s="10">
         <f t="shared" ref="D66:D70" si="14">_xlfn.XLOOKUP(A66,$A$2:$A$52,$N$2:$N$52)</f>
         <v>-311228.08999999997</v>
       </c>
@@ -4528,15 +5607,15 @@
       <c r="A67" t="s">
         <v>32</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="10">
         <f>_xlfn.XLOOKUP(A67,$A$1:$A$52,$D$1:$D$52)</f>
         <v>-149396.10000000987</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="10">
         <f t="shared" si="13"/>
         <v>-189254.06000000006</v>
       </c>
-      <c r="D67">
+      <c r="D67" s="10">
         <f t="shared" si="14"/>
         <v>-374962.91000000015</v>
       </c>
@@ -4545,15 +5624,15 @@
       <c r="A68" t="s">
         <v>38</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="10">
         <f t="shared" si="12"/>
         <v>-12230.810000000056</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="10">
         <f t="shared" si="13"/>
         <v>-45485.580000000075</v>
       </c>
-      <c r="D68">
+      <c r="D68" s="10">
         <f t="shared" si="14"/>
         <v>-72.879999999888241</v>
       </c>
@@ -4562,15 +5641,15 @@
       <c r="A69" t="s">
         <v>39</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="10">
         <f t="shared" si="12"/>
         <v>-4950.4699999999721</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="10">
         <f t="shared" si="13"/>
         <v>-8005.7900000010268</v>
       </c>
-      <c r="D69">
+      <c r="D69" s="10">
         <f t="shared" si="14"/>
         <v>-1724.9000000000233</v>
       </c>
@@ -4579,15 +5658,15 @@
       <c r="A70" t="s">
         <v>55</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="10">
         <f t="shared" si="12"/>
         <v>-184239.79000001028</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="10">
         <f t="shared" si="13"/>
         <v>-133456.33000001032</v>
       </c>
-      <c r="D70">
+      <c r="D70" s="10">
         <f t="shared" si="14"/>
         <v>-82077.349999999627</v>
       </c>
@@ -4615,15 +5694,15 @@
       <c r="A74" t="s">
         <v>24</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="10">
         <f>INDEX($D$2:$D$52, MATCH($A74,$A$2:$A$52))</f>
         <v>-36209.630000000005</v>
       </c>
-      <c r="C74">
+      <c r="C74" s="10">
         <f>INDEX($I$2:$I$52, MATCH($A74, $A$2:$A$52))</f>
         <v>-27292.159999999974</v>
       </c>
-      <c r="D74">
+      <c r="D74" s="10">
         <f>INDEX($N$2:$N$52, MATCH($A74,$A$2:$A$52))</f>
         <v>-9181.0800000000163</v>
       </c>
@@ -4632,15 +5711,15 @@
       <c r="A75" t="s">
         <v>25</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="10">
         <f t="shared" ref="B75:B79" si="15">INDEX($D$2:$D$52, MATCH($A75,$A$2:$A$52))</f>
         <v>0</v>
       </c>
-      <c r="C75">
+      <c r="C75" s="10">
         <f t="shared" ref="C75:C79" si="16">INDEX($I$2:$I$52, MATCH($A75, $A$2:$A$52))</f>
         <v>0</v>
       </c>
-      <c r="D75">
+      <c r="D75" s="10">
         <f t="shared" ref="D75:D79" si="17">INDEX($N$2:$N$52, MATCH($A75,$A$2:$A$52))</f>
         <v>-311228.08999999997</v>
       </c>
@@ -4649,15 +5728,15 @@
       <c r="A76" t="s">
         <v>32</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="10">
         <f t="shared" si="15"/>
         <v>-149396.10000000987</v>
       </c>
-      <c r="C76">
+      <c r="C76" s="10">
         <f t="shared" si="16"/>
         <v>-189254.06000000006</v>
       </c>
-      <c r="D76">
+      <c r="D76" s="10">
         <f t="shared" si="17"/>
         <v>-374962.91000000015</v>
       </c>
@@ -4666,15 +5745,15 @@
       <c r="A77" t="s">
         <v>38</v>
       </c>
-      <c r="B77">
+      <c r="B77" s="10">
         <f t="shared" si="15"/>
         <v>-12230.810000000056</v>
       </c>
-      <c r="C77">
+      <c r="C77" s="10">
         <f t="shared" si="16"/>
         <v>-45485.580000000075</v>
       </c>
-      <c r="D77">
+      <c r="D77" s="10">
         <f t="shared" si="17"/>
         <v>-72.879999999888241</v>
       </c>
@@ -4683,15 +5762,15 @@
       <c r="A78" t="s">
         <v>39</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="10">
         <f t="shared" si="15"/>
         <v>-4950.4699999999721</v>
       </c>
-      <c r="C78">
+      <c r="C78" s="10">
         <f t="shared" si="16"/>
         <v>-8005.7900000010268</v>
       </c>
-      <c r="D78">
+      <c r="D78" s="10">
         <f t="shared" si="17"/>
         <v>-1724.9000000000233</v>
       </c>
@@ -4700,15 +5779,15 @@
       <c r="A79" t="s">
         <v>55</v>
       </c>
-      <c r="B79">
+      <c r="B79" s="10">
         <f t="shared" si="15"/>
         <v>-184239.79000001028</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="10">
         <f t="shared" si="16"/>
         <v>-133456.33000001032</v>
       </c>
-      <c r="D79">
+      <c r="D79" s="10">
         <f t="shared" si="17"/>
         <v>-82077.349999999627</v>
       </c>
@@ -4735,22 +5814,40 @@
       <c r="A84" t="s">
         <v>73</v>
       </c>
-      <c r="B84" s="6"/>
-      <c r="C84" s="6"/>
+      <c r="B84" s="6">
+        <f>INDEX(Budget[FY17_Budget],MATCH(B87,Budget[Department]))</f>
+        <v>356640100</v>
+      </c>
+      <c r="C84" s="6">
+        <f>INDEX(Budget[FY17_Actual], MATCH(B87,Budget[Department]))</f>
+        <v>341243679.13</v>
+      </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>74</v>
       </c>
-      <c r="B85" s="6"/>
-      <c r="C85" s="6"/>
+      <c r="B85" s="6">
+        <f>INDEX(Budget[FY18_Budget],MATCH(B87,Budget[Department]))</f>
+        <v>382685200</v>
+      </c>
+      <c r="C85" s="6">
+        <f>INDEX(Budget[FY18_Actual], MATCH(B87,Budget[Department]))</f>
+        <v>346340810.81999999</v>
+      </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="6"/>
-      <c r="C86" s="6"/>
+      <c r="B86" s="6">
+        <f>INDEX(Budget[FY19_Budget],MATCH(B87,Budget[Department]))</f>
+        <v>376548600</v>
+      </c>
+      <c r="C86" s="6">
+        <f>INDEX(Budget[FY19_Actual], MATCH(B87,Budget[Department]))</f>
+        <v>355279492.22999901</v>
+      </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
@@ -4898,8 +5995,9 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>

<commit_message>
worked on the chart a little bit more. No clue on how to add the type of department in the bar graph.
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Barbie\Desktop\DA11\Excel\lookups-exercise-barbsjean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7575CEE5-C72E-43FA-B82C-778840869CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087BAAE3-04FA-4219-935D-9B5067627F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -953,7 +953,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -967,13 +967,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Budget</a:t>
+              <a:t>Budget Vs Actual</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Vs Actual</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -990,7 +985,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1028,13 +1023,42 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -1087,13 +1111,42 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -1146,13 +1199,42 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -1198,8 +1280,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
         <c:axId val="23809567"/>
         <c:axId val="312095903"/>
       </c:barChart>
@@ -1216,7 +1298,7 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -1426,12 +1508,9 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
@@ -1466,7 +1545,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="340">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1477,7 +1556,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -1490,7 +1569,7 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
@@ -1507,7 +1586,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1523,7 +1602,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -1567,35 +1646,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1607,30 +1686,31 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1732,14 +1812,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -1829,20 +1903,20 @@
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1855,6 +1929,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1886,7 +1971,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1895,14 +1980,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1956,14 +2040,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2353,7 +2431,7 @@
   <dimension ref="A1:P100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+      <selection activeCell="L85" sqref="L85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>